<commit_message>
Added new file. Minor edits.
</commit_message>
<xml_diff>
--- a/input_files/UC_case_study_5bus_network_C.xlsx
+++ b/input_files/UC_case_study_5bus_network_C.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus index" sheetId="5" r:id="rId1"/>
@@ -229,7 +229,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1953,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2088,7 +2087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2132,13 +2131,13 @@
       </c>
       <c r="C2" s="9">
         <f>(PI()/12)/(E2/100)*D2</f>
-        <v>3.4906585039886587E-3</v>
+        <v>2.6179938779914941E-3</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="F2" s="5">
         <v>0</v>
@@ -2153,13 +2152,13 @@
       </c>
       <c r="C3" s="9">
         <f>(PI()/12)/(E3/100)*D3</f>
-        <v>3.4906585039886587E-3</v>
+        <v>2.6179938779914941E-3</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
@@ -2409,7 +2408,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2643,19 +2642,19 @@
         <v>8</v>
       </c>
       <c r="E4" s="5">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="F4" s="5">
         <f>0.01*E4</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G4" s="5">
         <f>E4</f>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="H4" s="5">
         <f>G4</f>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="I4" s="5">
         <v>0</v>

</xml_diff>